<commit_message>
added example, profile on profile , valueset and codesystem
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="77">
   <si>
     <t>Path</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Extension</t>
+  </si>
+  <si>
+    <t>blah</t>
   </si>
   <si>
     <t/>
@@ -150,7 +153,7 @@
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
@@ -231,9 +234,6 @@
     <t>Extension.valueCode</t>
   </si>
   <si>
-    <t>valueCode</t>
-  </si>
-  <si>
     <t xml:space="preserve">code {[]} {[]}
 </t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>A bunch of example codes</t>
+  </si>
+  <si>
+    <t>http://www.fhir.org/guides/test3/ValueSet/blah-codes</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -432,7 +435,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="25.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.6015625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="53.8515625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
@@ -560,431 +563,431 @@
       <c r="A2" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>37</v>
+      </c>
       <c r="C2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE2" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s" s="2">
         <v>69</v>
       </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s" s="2">
         <v>70</v>
@@ -998,26 +1001,26 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W6" t="s" s="2">
         <v>73</v>
@@ -1026,40 +1029,40 @@
         <v>74</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to valid example
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -408,9 +408,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.53515625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.91015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.19921875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -418,7 +418,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="45.64453125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="42.953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -431,14 +431,14 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="25.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="53.8515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="24.68359375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="50.63671875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="18.25" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="17.44140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
updated to work ig tools added pages
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -150,7 +150,7 @@
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
@@ -164,7 +164,7 @@
     <t>xml:id (or equivalent in JSON)</t>
   </si>
   <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -184,10 +184,10 @@
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -209,7 +209,7 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t xml:space="preserve">null {[]} {[]}
+    <t xml:space="preserve">uri {[]} {[]}
 </t>
   </si>
   <si>
@@ -418,7 +418,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="42.953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.28515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
move toc back to breadcrumbs bar
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -157,7 +157,7 @@
     <t>Extension.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -180,7 +180,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -209,7 +209,7 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -222,7 +222,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.fhir.org/guides/test3/StructureDefinition/extension-blah"/&gt;</t>
+    <t>http://www.fhir.org/guides/test3/StructureDefinition/extension-blah</t>
   </si>
   <si>
     <t>N/A</t>
@@ -231,7 +231,7 @@
     <t>Extension.valueCode</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -303,67 +303,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>

</xml_diff>

<commit_message>
testing out new ig pub approach with templates
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$6</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="75">
   <si>
     <t>Path</t>
   </si>
@@ -239,16 +239,6 @@
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>valueCode</t>
   </si>
   <si>
     <t>required</t>
@@ -406,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1025,26 +1015,28 @@
         <v>37</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AB6" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>37</v>
+      </c>
       <c r="AC6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
         <v>68</v>
@@ -1065,110 +1057,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" hidden="true">
-      <c r="A7" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y7" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AJ7">
+  <autoFilter ref="A1:AJ6">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1178,7 +1068,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI6">
+  <conditionalFormatting sqref="A2:AI5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
play with yaml files
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$6</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="75">
   <si>
     <t>Path</t>
   </si>
@@ -239,16 +239,6 @@
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>valueCode</t>
   </si>
   <si>
     <t>required</t>
@@ -406,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1025,26 +1015,28 @@
         <v>37</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AB6" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>37</v>
+      </c>
       <c r="AC6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
         <v>68</v>
@@ -1065,110 +1057,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" hidden="true">
-      <c r="A7" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y7" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AJ7">
+  <autoFilter ref="A1:AJ6">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1178,7 +1068,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI6">
+  <conditionalFormatting sqref="A2:AI5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
test markdown in copyright
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -150,7 +150,7 @@
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
@@ -161,10 +161,10 @@
 </t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -184,10 +184,10 @@
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -238,7 +238,7 @@
     <t>Value of extension</t>
   </si>
   <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
+    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
   </si>
   <si>
     <t>required</t>
@@ -415,7 +415,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="42.953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.28515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>